<commit_message>
first version of sales summary agent
</commit_message>
<xml_diff>
--- a/store_sales_log.xlsx
+++ b/store_sales_log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Dev\agent-exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="186">
   <si>
     <t>Time</t>
   </si>
@@ -571,6 +574,12 @@
   </si>
   <si>
     <t>Biscuits</t>
+  </si>
+  <si>
+    <t>Chocolate</t>
+  </si>
+  <si>
+    <t>Detergent</t>
   </si>
 </sst>
 </file>
@@ -938,17 +947,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H181"/>
+  <dimension ref="A1:H183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G181"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4604,14 +4615,14 @@
         <v>6</v>
       </c>
       <c r="E131">
-        <f t="shared" ref="E131:E181" si="4">C131*D131</f>
+        <f t="shared" ref="E131:E183" si="4">C131*D131</f>
         <v>18</v>
       </c>
       <c r="F131">
         <v>4</v>
       </c>
       <c r="G131">
-        <f t="shared" ref="G131:G181" si="5">(D131-F131)*C131</f>
+        <f t="shared" ref="G131:G183" si="5">(D131-F131)*C131</f>
         <v>6</v>
       </c>
       <c r="H131">
@@ -6016,6 +6027,62 @@
       </c>
       <c r="H181">
         <v>171</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>165</v>
+      </c>
+      <c r="B182" t="s">
+        <v>184</v>
+      </c>
+      <c r="C182">
+        <v>0</v>
+      </c>
+      <c r="D182">
+        <v>2.5</v>
+      </c>
+      <c r="E182">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F182">
+        <v>1.5</v>
+      </c>
+      <c r="G182">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H182">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>165</v>
+      </c>
+      <c r="B183" t="s">
+        <v>185</v>
+      </c>
+      <c r="C183">
+        <v>0</v>
+      </c>
+      <c r="D183">
+        <v>7</v>
+      </c>
+      <c r="E183">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F183">
+        <v>5</v>
+      </c>
+      <c r="G183">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H183">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>